<commit_message>
refine printouts to include row numbers
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://internationalassociation162-my.sharepoint.com/personal/c_pettifor_iau-aiu_net/Documents/WHED/Australia/CRICOS-Import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="11_F25DC773A252ABDACC10486E81194A665ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD495851-AD57-43AA-9259-E74CDFFC0D5F}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="11_F25DC773A252ABDACC10486E81194A665ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EBD99A8-F7C5-4552-B45E-025D50309175}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="whed_levels" sheetId="4" r:id="rId1"/>
@@ -18,17 +18,28 @@
     <sheet name="ext_inst" sheetId="2" r:id="rId3"/>
     <sheet name="ext_cred" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
   <si>
     <t>Name English</t>
   </si>
@@ -96,9 +107,6 @@
     <t>Postal Address Postcode</t>
   </si>
   <si>
-    <t>Institution Type</t>
-  </si>
-  <si>
     <t>Institution ID</t>
   </si>
   <si>
@@ -229,6 +237,51 @@
   </si>
   <si>
     <t>Vocational Short Course</t>
+  </si>
+  <si>
+    <t>1 Smith Street</t>
+  </si>
+  <si>
+    <t>Pall Mall</t>
+  </si>
+  <si>
+    <t>South Kensington</t>
+  </si>
+  <si>
+    <t>SW11</t>
+  </si>
+  <si>
+    <t>Unit 1</t>
+  </si>
+  <si>
+    <t>Kensington</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Postal Address Country</t>
+  </si>
+  <si>
+    <t>Address Concat</t>
+  </si>
+  <si>
+    <t>Unit 1, 1 Smith Street, Pall Mall, South Kensington</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Row Index</t>
+  </si>
+  <si>
+    <t>Blue62</t>
+  </si>
+  <si>
+    <t>Acorn Institute</t>
+  </si>
+  <si>
+    <t>Oak Academy</t>
   </si>
 </sst>
 </file>
@@ -326,6 +379,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -593,7 +650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974E8CAB-D495-47CC-A487-D7F0464F0933}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -601,164 +658,164 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -768,15 +825,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:M1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -796,25 +853,49 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G2" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, H2:M2)</f>
+        <v>Unit 1, 1 Smith Street, Pall Mall, South Kensington Kensington SW11 Michigan Australia</v>
+      </c>
+      <c r="H2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -824,55 +905,97 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5C3BA5-4966-476E-B239-1E316FE5762C}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, G2:M2)</f>
+        <v>Unit 1 1 Smith Street Pall Mall South Kensington Kensington Michigan SW11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -892,46 +1015,46 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="O1" s="2"/>
     </row>

</xml_diff>

<commit_message>
initialise variables in whed_inst function
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://internationalassociation162-my.sharepoint.com/personal/c_pettifor_iau-aiu_net/Documents/WHED/Australia/CRICOS-Import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="11_F25DC773A252ABDACC10486E81194A665ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EBD99A8-F7C5-4552-B45E-025D50309175}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="11_F25DC773A252ABDACC10486E81194A665ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37C653DA-59FB-4107-8FA6-90803B08F9FB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="840" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="whed_levels" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="83">
   <si>
     <t>Name English</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>Oak Academy</t>
+  </si>
+  <si>
+    <t>IAU-000062</t>
+  </si>
+  <si>
+    <t>Acorn Institution</t>
   </si>
 </sst>
 </file>
@@ -827,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,6 +884,21 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
+        <v>80</v>
+      </c>
       <c r="G2" t="str">
         <f>_xlfn.TEXTJOIN(" ", TRUE, H2:M2)</f>
         <v>Unit 1, 1 Smith Street, Pall Mall, South Kensington Kensington SW11 Michigan Australia</v>
@@ -907,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5C3BA5-4966-476E-B239-1E316FE5762C}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add basic url tidy function and whed comparison
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://internationalassociation162-my.sharepoint.com/personal/c_pettifor_iau-aiu_net/Documents/WHED/Australia/CRICOS-Import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="11_F25DC773A252ABDACC10486E81194A665ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37C653DA-59FB-4107-8FA6-90803B08F9FB}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="11_F25DC773A252ABDACC10486E81194A665ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D6F1612-D20E-4C5C-B875-3989D3E95FF3}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="840" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -838,6 +838,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
continue work on creds & update template
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://internationalassociation162-my.sharepoint.com/personal/c_pettifor_iau-aiu_net/Documents/WHED/Australia/CRICOS-Import/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CraigPettifor\Documents\CRICOS-Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="11_F25DC773A252ABDACC10486E81194A665ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFB23CFB-7D57-42F3-8E06-8B6BE5CAB2C0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1A9CAA-F09E-46C6-93AE-043A09DC9094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="whed_levels" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
   <si>
     <t>Name English</t>
   </si>
@@ -297,6 +297,33 @@
   </si>
   <si>
     <t>whed_cred_name</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Bachelor of Computer Science</t>
+  </si>
+  <si>
+    <t>Red71</t>
+  </si>
+  <si>
+    <t>Bachelor of Informaticianistics</t>
+  </si>
+  <si>
+    <t>Orange31</t>
+  </si>
+  <si>
+    <t>Bachelor</t>
+  </si>
+  <si>
+    <t>02 - Information Technology</t>
+  </si>
+  <si>
+    <t>0201 - Computer Science</t>
+  </si>
+  <si>
+    <t>0208 - Informatician Mathmetician</t>
   </si>
 </sst>
 </file>
@@ -396,10 +423,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -667,11 +690,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974E8CAB-D495-47CC-A487-D7F0464F0933}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -919,6 +947,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1013,10 +1043,16 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -1110,13 +1146,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D569F62-FAA7-470F-8473-61A4FFD6C92E}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -1162,6 +1214,58 @@
         <v>34</v>
       </c>
       <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>